<commit_message>
calculate error of g
</commit_message>
<xml_diff>
--- a/Experiments/raw_data_modified.xlsx
+++ b/Experiments/raw_data_modified.xlsx
@@ -2,19 +2,19 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="U:\Data_git\Data_Analysis\Experiments\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\98415\Data_Analysis\Experiments\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17250" windowHeight="5895"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="5892"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="25">
   <si>
     <t>distance</t>
   </si>
@@ -100,23 +100,39 @@
   </si>
   <si>
     <t>mean_dis</t>
+  </si>
+  <si>
+    <t>g</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>mean_g</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>time</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>standard_error</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="9"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -142,15 +158,21 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="常规" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -428,27 +450,27 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M12"/>
+  <dimension ref="A1:M16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+      <selection activeCell="M11" sqref="M11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.85546875" customWidth="1"/>
+    <col min="1" max="1" width="16.88671875" customWidth="1"/>
     <col min="2" max="2" width="11" customWidth="1"/>
-    <col min="8" max="8" width="9.28515625" customWidth="1"/>
-    <col min="9" max="9" width="11.42578125" customWidth="1"/>
-    <col min="10" max="10" width="10.42578125" customWidth="1"/>
-    <col min="11" max="11" width="10.85546875" customWidth="1"/>
-    <col min="12" max="12" width="16.7109375" customWidth="1"/>
-    <col min="13" max="13" width="14.28515625" customWidth="1"/>
-    <col min="14" max="14" width="16.28515625" customWidth="1"/>
-    <col min="15" max="15" width="12.42578125" customWidth="1"/>
+    <col min="8" max="8" width="9.33203125" customWidth="1"/>
+    <col min="9" max="9" width="11.44140625" customWidth="1"/>
+    <col min="10" max="10" width="10.44140625" customWidth="1"/>
+    <col min="11" max="11" width="10.88671875" customWidth="1"/>
+    <col min="12" max="12" width="16.6640625" customWidth="1"/>
+    <col min="13" max="13" width="14.33203125" customWidth="1"/>
+    <col min="14" max="14" width="16.33203125" customWidth="1"/>
+    <col min="15" max="15" width="12.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>2</v>
       </c>
@@ -468,7 +490,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:13">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -506,7 +528,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:13">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>10</v>
       </c>
@@ -547,7 +569,7 @@
         <v>4.0496913462636654E-5</v>
       </c>
     </row>
-    <row r="4" spans="1:13">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>
       <c r="B4">
         <v>0.29086000000000001</v>
@@ -586,7 +608,7 @@
         <v>2.0093421809139421E-3</v>
       </c>
     </row>
-    <row r="5" spans="1:13">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
       <c r="B5">
         <v>0.29093999999999998</v>
@@ -625,7 +647,7 @@
         <v>1.2158947322856971E-4</v>
       </c>
     </row>
-    <row r="6" spans="1:13">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" s="1"/>
       <c r="B6">
         <v>0.29104000000000002</v>
@@ -664,7 +686,7 @@
         <v>8.376156636548763E-5</v>
       </c>
     </row>
-    <row r="7" spans="1:13">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" s="1"/>
       <c r="B7">
         <v>0.29083999999999999</v>
@@ -703,7 +725,7 @@
         <v>1.9390719429671539E-5</v>
       </c>
     </row>
-    <row r="8" spans="1:13">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>7</v>
       </c>
@@ -728,53 +750,46 @@
         <v>0.29520599999999997</v>
       </c>
     </row>
-    <row r="9" spans="1:13">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="B9">
+        <f>2*B2/B8^2</f>
         <v>9.675107992828627</v>
       </c>
       <c r="C9">
+        <f t="shared" ref="C9:F9" si="3">2*C2/C8^2</f>
         <v>9.7765830816769288</v>
       </c>
       <c r="D9">
+        <f t="shared" si="3"/>
         <v>9.884552669151434</v>
       </c>
       <c r="E9">
+        <f t="shared" si="3"/>
         <v>9.8797480052495743</v>
       </c>
       <c r="F9">
+        <f t="shared" si="3"/>
         <v>9.9712458677098414</v>
       </c>
       <c r="J9" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:13">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B10">
-        <f>((B3-B8)^2+(B4-B8)^2+(B5-B8)^2+(B6-B8)^2+(B7-B8)^2)/(5-1)</f>
-        <v>8.2000000000014135E-9</v>
-      </c>
-      <c r="C10">
-        <f>((C3-C8)^2+(C4-C8)^2+(C5-C8)^2+(C6-C8)^2+(C7-C8)^2)/(5-1)</f>
-        <v>2.0187279999999994E-5</v>
-      </c>
-      <c r="D10">
-        <f>((D3-D8)^2+(D4-D8)^2+(D5-D8)^2+(D6-D8)^2+(D7-D8)^2)/(5-1)</f>
-        <v>7.3920000000005363E-8</v>
-      </c>
-      <c r="E10">
-        <f>((E3-E8)^2+(E4-E8)^2+(E5-E8)^2+(E6-E8)^2+(E7-E8)^2)/(5-1)</f>
-        <v>3.5079999999999941E-8</v>
-      </c>
-      <c r="F10">
-        <f>((F3-F8)^2+(F4-F8)^2+(F5-F8)^2+(F6-F8)^2+(F7-F8)^2)/(5-1)</f>
-        <v>1.880000000001207E-9</v>
-      </c>
+        <v>22</v>
+      </c>
+      <c r="B10" s="4">
+        <f>AVERAGE(B9:F9)</f>
+        <v>9.8374475233232808</v>
+      </c>
+      <c r="C10" s="4"/>
+      <c r="D10" s="4"/>
+      <c r="E10" s="4"/>
+      <c r="F10" s="4"/>
       <c r="J10" t="s">
         <v>20</v>
       </c>
@@ -788,25 +803,18 @@
         <v>18</v>
       </c>
     </row>
-    <row r="11" spans="1:13">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="B11">
-        <v>9.0553851381381965E-5</v>
-      </c>
-      <c r="C11">
-        <v>4.4930257065812556E-3</v>
-      </c>
-      <c r="D11">
-        <v>2.7188232748747272E-4</v>
-      </c>
-      <c r="E11">
-        <v>1.8729655629509033E-4</v>
-      </c>
-      <c r="F11">
-        <v>4.3358966777371517E-5</v>
-      </c>
+        <v>13</v>
+      </c>
+      <c r="B11" s="4">
+        <f>STDEVP(B9:F9)</f>
+        <v>0.10194981698210133</v>
+      </c>
+      <c r="C11" s="4"/>
+      <c r="D11" s="4"/>
+      <c r="E11" s="4"/>
+      <c r="F11" s="4"/>
       <c r="J11">
         <f>AVERAGE(H3:H7)</f>
         <v>0.40687999999999996</v>
@@ -824,27 +832,100 @@
         <v>7.9158069708653162E-3</v>
       </c>
     </row>
-    <row r="12" spans="1:13">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B12" s="4">
+        <f>B11/SQRT(5)</f>
+        <v>4.5593344213128204E-2</v>
+      </c>
+      <c r="C12" s="4"/>
+      <c r="D12" s="4"/>
+      <c r="E12" s="4"/>
+      <c r="F12" s="4"/>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B13" s="3"/>
+      <c r="C13" s="3"/>
+      <c r="D13" s="3"/>
+      <c r="E13" s="3"/>
+      <c r="F13" s="3"/>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B14">
+        <f>((B3-B8)^2+(B4-B8)^2+(B5-B8)^2+(B6-B8)^2+(B7-B8)^2)/(5-1)</f>
+        <v>8.2000000000014135E-9</v>
+      </c>
+      <c r="C14">
+        <f>((C3-C8)^2+(C4-C8)^2+(C5-C8)^2+(C6-C8)^2+(C7-C8)^2)/(5-1)</f>
+        <v>2.0187279999999994E-5</v>
+      </c>
+      <c r="D14">
+        <f>((D3-D8)^2+(D4-D8)^2+(D5-D8)^2+(D6-D8)^2+(D7-D8)^2)/(5-1)</f>
+        <v>7.3920000000005363E-8</v>
+      </c>
+      <c r="E14">
+        <f>((E3-E8)^2+(E4-E8)^2+(E5-E8)^2+(E6-E8)^2+(E7-E8)^2)/(5-1)</f>
+        <v>3.5079999999999941E-8</v>
+      </c>
+      <c r="F14">
+        <f>((F3-F8)^2+(F4-F8)^2+(F5-F8)^2+(F6-F8)^2+(F7-F8)^2)/(5-1)</f>
+        <v>1.880000000001207E-9</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B15">
+        <v>9.0553851381381965E-5</v>
+      </c>
+      <c r="C15">
+        <v>4.4930257065812556E-3</v>
+      </c>
+      <c r="D15">
+        <v>2.7188232748747272E-4</v>
+      </c>
+      <c r="E15">
+        <v>1.8729655629509033E-4</v>
+      </c>
+      <c r="F15">
+        <v>4.3358966777371517E-5</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B12">
+      <c r="B16">
         <v>4.0496913462636661E-5</v>
       </c>
-      <c r="C12">
+      <c r="C16">
         <v>2.0093421809139421E-3</v>
       </c>
-      <c r="D12">
+      <c r="D16">
         <v>1.2158947322856971E-4</v>
       </c>
-      <c r="E12">
+      <c r="E16">
         <v>8.376156636548763E-5</v>
       </c>
-      <c r="F12">
+      <c r="F16">
         <v>1.9390719429671539E-5</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="B10:F10"/>
+    <mergeCell ref="B11:F11"/>
+    <mergeCell ref="B12:F12"/>
+  </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>